<commit_message>
Scenarij 2 nešto nešto, bit će promjene
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/Scenarij/S2-UnosHotela.xlsx
+++ b/UseCaseIScenarij/Scenarij/S2-UnosHotela.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t xml:space="preserve">Naziv </t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>Admin je logovan</t>
+  </si>
+  <si>
+    <t>Neuspješno kreiranje</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>1.već je nekom drugom hotelu menadžer</t>
+  </si>
+  <si>
+    <t>2.Odabira drugog menadžera</t>
   </si>
 </sst>
 </file>
@@ -217,15 +229,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -242,15 +245,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -536,7 +548,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,152 +562,172 @@
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="6"/>
     </row>
     <row r="14" spans="1:3" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="8"/>
     </row>
     <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="9" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="7"/>
+      <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10" t="s">
+    <row r="19" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="10"/>
-    </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-    </row>
-    <row r="22" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:2" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:2" ht="29.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:2" ht="52" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:3" ht="29.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:3" ht="52" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B7:C7"/>

</xml_diff>